<commit_message>
created bom for remaining container 03 buildout, internal use
</commit_message>
<xml_diff>
--- a/prj/fs-rack/v2.0/fs_rack_bom_2.0.xlsx
+++ b/prj/fs-rack/v2.0/fs_rack_bom_2.0.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsavas/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsavas/Documents/git/openag-mechanical/prj/fs-rack/v2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6C291A6F-4989-A245-8F6E-89F9D8A892C7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{182C0AED-D212-C640-8E25-1B23AB07D4AA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_fs_rack_bom" sheetId="2" r:id="rId1"/>
-    <sheet name="_meta" sheetId="4" r:id="rId2"/>
+    <sheet name="container03" sheetId="5" r:id="rId2"/>
+    <sheet name="_meta" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="77">
   <si>
     <t>Part</t>
   </si>
@@ -246,6 +247,12 @@
   </si>
   <si>
     <t>Contained in this file is the current, stable bill of materials for the latest version of the OpenAg Initiative Food Server's™ hydroponic rack system. This version of the rack system includes several mechanical changes: removal of hydroponic reservoir, effective connections to Waterbot, addition of mixing chamber, sensor probe mounting, and others. Bom will be updated with remaining components shortly.</t>
+  </si>
+  <si>
+    <t>Adding new column for 6 units</t>
+  </si>
+  <si>
+    <t>For 6</t>
   </si>
 </sst>
 </file>
@@ -255,7 +262,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -283,8 +290,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +324,16 @@
         <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -313,10 +344,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -344,7 +377,6 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -355,8 +387,44 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -673,28 +741,28 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="41.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.5" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" customWidth="1"/>
-    <col min="9" max="10" width="16.5" customWidth="1"/>
-    <col min="11" max="16384" width="14.5" hidden="1"/>
+    <col min="3" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+    <col min="10" max="11" width="16.5" customWidth="1"/>
+    <col min="12" max="16384" width="14.5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -704,29 +772,32 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -734,29 +805,36 @@
       <c r="C2" s="7">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7">
+        <f>C2*6</f>
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="8" t="str">
+      <c r="F2" s="8" t="str">
         <f>HYPERLINK("https://www.amazon.com/KingSo-Irrigation-Venturi-Fertilizer-Watering/dp/B07C2K6JQ4/ref=sr_1_3?ie=UTF8&amp;qid=1526909082&amp;sr=8-3&amp;keywords=1%2F2%22+venturi","Amazon")</f>
         <v>Amazon</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="10">
+      <c r="H2" s="10">
         <v>19.440000000000001</v>
       </c>
-      <c r="H2" s="11"/>
       <c r="I2" s="12">
+        <f>H2*C2</f>
+        <v>19.440000000000001</v>
+      </c>
+      <c r="J2" s="11">
         <v>0.41</v>
       </c>
-      <c r="J2" s="12">
-        <f>C2*I2</f>
+      <c r="K2" s="11">
+        <f>C2*J2</f>
         <v>0.41</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -764,31 +842,35 @@
       <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D25" si="0">C3*6</f>
+        <v>6</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="10">
+      <c r="H3" s="10">
         <v>89.99</v>
       </c>
-      <c r="H3" s="13">
-        <f>G3*C3</f>
+      <c r="I3" s="12">
+        <f>H3*C3</f>
         <v>89.99</v>
       </c>
-      <c r="I3" s="12">
+      <c r="J3" s="11">
         <v>10.8</v>
       </c>
-      <c r="J3" s="12">
-        <f>C3*I3</f>
+      <c r="K3" s="11">
+        <f>C3*J3</f>
         <v>10.8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -798,32 +880,36 @@
       <c r="C4" s="7">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8" t="str">
+      <c r="F4" s="8" t="str">
         <f>HYPERLINK("https://www.grainger.com/product/LASCO-PVC-Tee-22FL01","Grainger")</f>
         <v>Grainger</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="10">
+      <c r="H4" s="10">
         <v>1.23</v>
       </c>
-      <c r="H4" s="13">
-        <f>G4*C4</f>
+      <c r="I4" s="12">
+        <f>H4*C4</f>
         <v>2.46</v>
       </c>
-      <c r="I4" s="12">
+      <c r="J4" s="11">
         <v>0.1</v>
       </c>
-      <c r="J4" s="12">
-        <f>C4*I4</f>
+      <c r="K4" s="11">
+        <f>C4*J4</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
@@ -833,31 +919,35 @@
       <c r="C5" s="7">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="8" t="str">
+      <c r="F5" s="8" t="str">
         <f>HYPERLINK("https://www.grainger.com/product/LASCO-PVC-Male-Adapter-22FJ19","Grainger")</f>
         <v>Grainger</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="10">
+      <c r="H5" s="10">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H5" s="13">
+      <c r="I5" s="12">
         <v>11.36</v>
       </c>
-      <c r="I5" s="12">
+      <c r="J5" s="11">
         <v>0.03</v>
       </c>
-      <c r="J5" s="12">
-        <f>C5*I5</f>
+      <c r="K5" s="11">
+        <f>C5*J5</f>
         <v>0.06</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -867,32 +957,36 @@
       <c r="C6" s="7">
         <v>2</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="8" t="str">
+      <c r="F6" s="8" t="str">
         <f>HYPERLINK("https://www.grainger.com/product/LASCO-PVC-Elbow-22FJ74?cm_sp=Home-_-MyPurchasedProducts-_-22FJ74&amp;cm_vc=HPMPPZ","Grainger")</f>
         <v>Grainger</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="10">
+      <c r="H6" s="10">
         <v>0.66</v>
       </c>
-      <c r="H6" s="13">
-        <f>G6*C6</f>
+      <c r="I6" s="12">
+        <f>H6*C6</f>
         <v>1.32</v>
       </c>
-      <c r="I6" s="12">
+      <c r="J6" s="11">
         <v>0.05</v>
       </c>
-      <c r="J6" s="12">
-        <f>C6*I6</f>
+      <c r="K6" s="11">
+        <f>C6*J6</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
@@ -902,31 +996,35 @@
       <c r="C7" s="7">
         <v>1</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="8" t="str">
+      <c r="F7" s="8" t="str">
         <f>HYPERLINK("https://www.grainger.com/product/LASCO-PVC-Union-22FM79","Grainger")</f>
         <v>Grainger</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="G7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="10">
+      <c r="H7" s="10">
         <v>2.78</v>
       </c>
-      <c r="H7" s="13">
+      <c r="I7" s="12">
         <v>11.36</v>
       </c>
-      <c r="I7" s="12">
+      <c r="J7" s="11">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J7" s="12">
-        <f>C7*I7</f>
+      <c r="K7" s="11">
+        <f>C7*J7</f>
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -936,32 +1034,36 @@
       <c r="C8" s="7">
         <v>2</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="8" t="str">
+      <c r="F8" s="8" t="str">
         <f>HYPERLINK("https://www.grainger.com/product/LASCO-PVC-Street-Elbow-22FJ98","Grainger")</f>
         <v>Grainger</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="10">
+      <c r="H8" s="10">
         <v>0.97</v>
       </c>
-      <c r="H8" s="13">
-        <f>G8*C8</f>
+      <c r="I8" s="12">
+        <f>H8*C8</f>
         <v>1.94</v>
       </c>
-      <c r="I8" s="12">
+      <c r="J8" s="11">
         <v>0.05</v>
       </c>
-      <c r="J8" s="12">
-        <f>C8*I8</f>
+      <c r="K8" s="11">
+        <f>C8*J8</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
         <v>31</v>
       </c>
@@ -971,32 +1073,36 @@
       <c r="C9" s="7">
         <v>2</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="8" t="str">
+      <c r="F9" s="8" t="str">
         <f>HYPERLINK("https://www.grainger.com/product/LASCO-PVC-Union-22FM80","Grainger")</f>
         <v>Grainger</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="10">
+      <c r="H9" s="10">
         <v>4.5</v>
       </c>
-      <c r="H9" s="13">
-        <f>C9*G9</f>
+      <c r="I9" s="12">
+        <f>C9*H9</f>
         <v>9</v>
       </c>
-      <c r="I9" s="12">
+      <c r="J9" s="11">
         <v>0.2</v>
       </c>
-      <c r="J9" s="12">
-        <f>C9*I9</f>
+      <c r="K9" s="11">
+        <f>C9*J9</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -1004,32 +1110,36 @@
       <c r="C10" s="7">
         <v>2</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="8" t="str">
+      <c r="F10" s="8" t="str">
         <f>HYPERLINK("https://www.grainger.com/product/GF-PIPING-SYSTEMS-PVC-Union-11W267","Grainger")</f>
         <v>Grainger</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="10">
+      <c r="H10" s="10">
         <v>5.97</v>
       </c>
-      <c r="H10" s="13">
-        <f>C10*G10</f>
+      <c r="I10" s="12">
+        <f>C10*H10</f>
         <v>11.94</v>
       </c>
-      <c r="I10" s="12">
+      <c r="J10" s="11">
         <v>0.11</v>
       </c>
-      <c r="J10" s="12">
-        <f>C10*I10</f>
+      <c r="K10" s="11">
+        <f>C10*J10</f>
         <v>0.22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
         <v>36</v>
       </c>
@@ -1039,27 +1149,31 @@
       <c r="C11" s="7">
         <v>1</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="8" t="str">
+      <c r="F11" s="8" t="str">
         <f>HYPERLINK("https://www.homedepot.com/p/1-2-in-Compression-x-1-2-in-FIP-x-12-in-Braided-Polymer-Faucet-Connector-B3-12A-F/100143862","Home Depot")</f>
         <v>Home Depot</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="10">
+      <c r="H11" s="10">
         <v>5.98</v>
       </c>
-      <c r="H11" s="13">
-        <f>G11*C11</f>
+      <c r="I11" s="12">
+        <f>H11*C11</f>
         <v>5.98</v>
       </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-    </row>
-    <row r="12" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
         <v>39</v>
       </c>
@@ -1069,27 +1183,31 @@
       <c r="C12" s="7">
         <v>1</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="8" t="str">
+      <c r="F12" s="8" t="str">
         <f>HYPERLINK("https://www.homedepot.com/p/BrassCraft-1-2-in-Compression-x-1-2-in-FIP-x-16-in-Braided-Polymer-Faucet-Connector-B3-16A-F/100148838","Home Depot")</f>
         <v>Home Depot</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="10">
+      <c r="H12" s="10">
         <v>6.47</v>
       </c>
-      <c r="H12" s="13">
-        <f>G12*C12</f>
+      <c r="I12" s="12">
+        <f>H12*C12</f>
         <v>6.47</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-    </row>
-    <row r="13" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
         <v>41</v>
       </c>
@@ -1099,32 +1217,36 @@
       <c r="C13" s="7">
         <v>1</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="8" t="str">
+      <c r="F13" s="8" t="str">
         <f>HYPERLINK("https://www.homedepot.com/p/Everbilt-1-2-in-x-1-4-in-Brass-MPT-x-MHT-Boiler-Drain-VBDQTRC3EB/205811822","Home Depot")</f>
         <v>Home Depot</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="10">
+      <c r="H13" s="10">
         <v>8.9</v>
       </c>
-      <c r="H13" s="13">
-        <f>G13*C13</f>
+      <c r="I13" s="12">
+        <f>H13*C13</f>
         <v>8.9</v>
       </c>
-      <c r="I13" s="12">
+      <c r="J13" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J13" s="12">
-        <f>C13*I13</f>
+      <c r="K13" s="11">
+        <f>C13*J13</f>
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
@@ -1132,32 +1254,36 @@
       <c r="C14" s="7">
         <v>1</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="8" t="str">
+      <c r="F14" s="8" t="str">
         <f>HYPERLINK("https://www.homedepot.com/p/Simpson-Strong-Tie-ZMAX-18-Gauge-Galvanized-Steel-Angle-A21Z/100375047","Home Depot")</f>
         <v>Home Depot</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="G14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="10">
+      <c r="H14" s="10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H14" s="13">
-        <f>C14*G14</f>
+      <c r="I14" s="12">
+        <f>C14*H14</f>
         <v>0.57999999999999996</v>
       </c>
-      <c r="I14" s="12">
+      <c r="J14" s="11">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="J14" s="12">
-        <f>C14*I14</f>
+      <c r="K14" s="11">
+        <f>C14*J14</f>
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
         <v>47</v>
       </c>
@@ -1167,32 +1293,36 @@
       <c r="C15" s="7">
         <v>1</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="8" t="str">
+      <c r="F15" s="8" t="str">
         <f>HYPERLINK("https://www.matcodist.com/plant-distribution-cartindustrial-rolling-rack-horticulture-cart-nursery-cartplant-cart-flower-cart-greenhouse-transportation-cart","Matco")</f>
         <v>Matco</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="G15" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="10">
+      <c r="H15" s="10">
         <v>237</v>
       </c>
-      <c r="H15" s="13">
-        <f>G15*C15</f>
+      <c r="I15" s="12">
+        <f>H15*C15</f>
         <v>237</v>
       </c>
-      <c r="I15" s="12">
+      <c r="J15" s="11">
         <v>60</v>
       </c>
-      <c r="J15" s="12">
-        <f>C15*I15</f>
+      <c r="K15" s="11">
+        <f>C15*J15</f>
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
         <v>50</v>
       </c>
@@ -1202,31 +1332,35 @@
       <c r="C16" s="7">
         <v>2</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="8" t="str">
+      <c r="F16" s="8" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/#4061t163/=1afszoi","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="G16" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="10">
+      <c r="H16" s="10">
         <v>11.36</v>
       </c>
-      <c r="H16" s="13">
+      <c r="I16" s="12">
         <v>11.36</v>
       </c>
-      <c r="I16" s="12">
+      <c r="J16" s="11">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="J16" s="12">
-        <f>C16*I16</f>
+      <c r="K16" s="11">
+        <f>C16*J16</f>
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
         <v>52</v>
       </c>
@@ -1236,32 +1370,36 @@
       <c r="C17" s="7">
         <v>2</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="8" t="str">
+      <c r="F17" s="8" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/#3185k112/=1aft071","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="G17" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="10">
+      <c r="H17" s="10">
         <v>0.44</v>
       </c>
-      <c r="H17" s="13">
-        <f>G17*C17</f>
+      <c r="I17" s="12">
+        <f>H17*C17</f>
         <v>0.88</v>
       </c>
-      <c r="I17" s="12">
+      <c r="J17" s="11">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J17" s="12">
-        <f>C17*I17</f>
+      <c r="K17" s="11">
+        <f>C17*J17</f>
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>54</v>
       </c>
@@ -1271,32 +1409,36 @@
       <c r="C18" s="7">
         <v>1</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="8" t="str">
+      <c r="F18" s="8" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/#9930k63/=1aft65a","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="G18" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="10">
+      <c r="H18" s="10">
         <v>214.79</v>
       </c>
-      <c r="H18" s="13">
-        <f>C18*G18</f>
+      <c r="I18" s="12">
+        <f>C18*H18</f>
         <v>214.79</v>
       </c>
-      <c r="I18" s="12">
+      <c r="J18" s="11">
         <v>8.4</v>
       </c>
-      <c r="J18" s="12">
-        <f>C18*I18</f>
+      <c r="K18" s="11">
+        <f>C18*J18</f>
         <v>8.4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
         <v>57</v>
       </c>
@@ -1306,27 +1448,31 @@
       <c r="C19" s="7">
         <v>3</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="8" t="str">
+      <c r="F19" s="8" t="str">
         <f>HYPERLINK("https://www.mscdirect.com/product/details/08802845","MSCDirect")</f>
         <v>MSCDirect</v>
       </c>
-      <c r="F19" s="9">
+      <c r="G19" s="9">
         <v>8802845</v>
       </c>
-      <c r="G19" s="10">
+      <c r="H19" s="10">
         <v>0.79</v>
       </c>
-      <c r="H19" s="13">
-        <f>G19*C19</f>
+      <c r="I19" s="12">
+        <f>H19*C19</f>
         <v>2.37</v>
       </c>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+    </row>
+    <row r="20" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
         <v>59</v>
       </c>
@@ -1336,27 +1482,31 @@
       <c r="C20" s="7">
         <v>1</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="8" t="str">
+      <c r="F20" s="8" t="str">
         <f>HYPERLINK("https://www.mscdirect.com/product/details/05726468","MSCDirect")</f>
         <v>MSCDirect</v>
       </c>
-      <c r="F20" s="9">
+      <c r="G20" s="9">
         <v>5726468</v>
       </c>
-      <c r="G20" s="10">
+      <c r="H20" s="10">
         <v>0.85</v>
       </c>
-      <c r="H20" s="13">
-        <f>G20*C20</f>
+      <c r="I20" s="12">
+        <f>H20*C20</f>
         <v>0.85</v>
       </c>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+    </row>
+    <row r="21" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
         <v>60</v>
       </c>
@@ -1366,26 +1516,30 @@
       <c r="C21" s="7">
         <v>1</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="8" t="str">
+      <c r="F21" s="8" t="str">
         <f>HYPERLINK("https://www.mscdirect.com/product/details/08803066","MSCDirect")</f>
         <v>MSCDirect</v>
       </c>
-      <c r="F21" s="9">
+      <c r="G21" s="9">
         <v>8803066</v>
       </c>
-      <c r="G21" s="10">
+      <c r="H21" s="10">
         <v>0.8</v>
       </c>
-      <c r="H21" s="13">
+      <c r="I21" s="12">
         <v>11.36</v>
       </c>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+    </row>
+    <row r="22" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
         <v>61</v>
       </c>
@@ -1395,27 +1549,31 @@
       <c r="C22" s="7">
         <v>1</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="8" t="str">
+      <c r="F22" s="8" t="str">
         <f>HYPERLINK("https://www.mscdirect.com/product/details/50580885","MSCDirect")</f>
         <v>MSCDirect</v>
       </c>
-      <c r="F22" s="9">
+      <c r="G22" s="9">
         <v>50580885</v>
       </c>
-      <c r="G22" s="10">
+      <c r="H22" s="10">
         <v>0.99</v>
       </c>
-      <c r="H22" s="13">
-        <f>G22*C22</f>
+      <c r="I22" s="12">
+        <f>H22*C22</f>
         <v>0.99</v>
       </c>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+    </row>
+    <row r="23" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
         <v>63</v>
       </c>
@@ -1425,30 +1583,34 @@
       <c r="C23" s="7">
         <v>3</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="8" t="str">
+      <c r="F23" s="8" t="str">
         <f>HYPERLINK("https://www.mscdirect.com/product/details/08802852","MSCDirect")</f>
         <v>MSCDirect</v>
       </c>
-      <c r="F23" s="9">
+      <c r="G23" s="9">
         <v>8802852</v>
       </c>
-      <c r="G23" s="10">
+      <c r="H23" s="10">
         <v>0.85</v>
       </c>
-      <c r="H23" s="13">
-        <f>C23*G23</f>
+      <c r="I23" s="12">
+        <f>C23*H23</f>
         <v>2.5499999999999998</v>
       </c>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12">
-        <f>C23*I23</f>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11">
+        <f>C23*J23</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
         <v>64</v>
       </c>
@@ -1458,32 +1620,36 @@
       <c r="C24" s="7">
         <v>1</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="8" t="str">
+      <c r="F24" s="8" t="str">
         <f>HYPERLINK("https://www.mscdirect.com/product/details/05726484","MSCDirect")</f>
         <v>MSCDirect</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G24" s="10">
+      <c r="H24" s="10">
         <v>1.05</v>
       </c>
-      <c r="H24" s="13">
-        <f>C24*G24</f>
+      <c r="I24" s="12">
+        <f>C24*H24</f>
         <v>1.05</v>
       </c>
-      <c r="I24" s="12">
+      <c r="J24" s="11">
         <v>0.18</v>
       </c>
-      <c r="J24" s="12">
-        <f>C24*I24</f>
+      <c r="K24" s="11">
+        <f>C24*J24</f>
         <v>0.18</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
         <v>66</v>
       </c>
@@ -1491,84 +1657,1049 @@
       <c r="C25" s="7">
         <v>1</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="F25" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="G25" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G25" s="10">
+      <c r="H25" s="10">
         <v>73.87</v>
       </c>
-      <c r="H25" s="13">
-        <f>C25*G25</f>
+      <c r="I25" s="12">
+        <f>C25*H25</f>
         <v>73.87</v>
       </c>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-    </row>
-    <row r="26" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+    </row>
+    <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="str">
         <f>HYPERLINK("https://www.mscdirect.com/product/details/67725085","#6 standoffs")</f>
         <v>#6 standoffs</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="13"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="10"/>
       <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-    </row>
-    <row r="27" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+    </row>
+    <row r="27" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="13"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="10"/>
       <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-    </row>
-    <row r="28" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+    </row>
+    <row r="28" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="13"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="10"/>
       <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://www.amazon.com/dp/B00CJIBMIK/ref=asc_df_B00CJIBMIK5482529/?tag=hyprod-20&amp;creative=394997&amp;creativeASIN=B00CJIBMIK&amp;linkCode=df0&amp;hvadid=167148561991&amp;hvpos=1o1&amp;hvnetw=g&amp;hvrand=6662302602102131996&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9001933&amp;hvtargid=pla-307268360582" xr:uid="{C5874CC2-E8EF-2445-986A-129CA96EED95}"/>
+    <hyperlink ref="F3" r:id="rId1" display="https://www.amazon.com/dp/B00CJIBMIK/ref=asc_df_B00CJIBMIK5482529/?tag=hyprod-20&amp;creative=394997&amp;creativeASIN=B00CJIBMIK&amp;linkCode=df0&amp;hvadid=167148561991&amp;hvpos=1o1&amp;hvnetw=g&amp;hvrand=6662302602102131996&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9001933&amp;hvtargid=pla-307268360582" xr:uid="{C5874CC2-E8EF-2445-986A-129CA96EED95}"/>
   </hyperlinks>
-  <printOptions horizontalCentered="1" gridLines="1"/>
+  <printOptions horizontalCentered="1" headings="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
   <ignoredErrors>
-    <ignoredError sqref="F13 F24" numberStoredAsText="1"/>
-    <ignoredError sqref="H14 H18" formula="1"/>
+    <ignoredError sqref="G13 G24" numberStoredAsText="1"/>
+    <ignoredError sqref="I14 I18" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCBFFEC-9DF1-E041-9D20-25D315E3E8C4}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="41.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+    <col min="10" max="11" width="16.5" customWidth="1"/>
+    <col min="12" max="16384" width="14.5" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26">
+        <v>1</v>
+      </c>
+      <c r="D2" s="26">
+        <f>C2*6</f>
+        <v>6</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="27" t="str">
+        <f>HYPERLINK("https://www.amazon.com/KingSo-Irrigation-Venturi-Fertilizer-Watering/dp/B07C2K6JQ4/ref=sr_1_3?ie=UTF8&amp;qid=1526909082&amp;sr=8-3&amp;keywords=1%2F2%22+venturi","Amazon")</f>
+        <v>Amazon</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="29">
+        <v>19.440000000000001</v>
+      </c>
+      <c r="I2" s="27">
+        <f>H2*C2</f>
+        <v>19.440000000000001</v>
+      </c>
+      <c r="J2" s="30">
+        <v>0.41</v>
+      </c>
+      <c r="K2" s="30">
+        <f>C2*J2</f>
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="19">
+        <v>1</v>
+      </c>
+      <c r="D3" s="19">
+        <f t="shared" ref="D3:D24" si="0">C3*6</f>
+        <v>6</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="22">
+        <v>89.99</v>
+      </c>
+      <c r="I3" s="20">
+        <f>H3*C3</f>
+        <v>89.99</v>
+      </c>
+      <c r="J3" s="23">
+        <v>10.8</v>
+      </c>
+      <c r="K3" s="23">
+        <f>C3*J3</f>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="19">
+        <v>2</v>
+      </c>
+      <c r="D4" s="19">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="20" t="str">
+        <f>HYPERLINK("https://www.grainger.com/product/LASCO-PVC-Tee-22FL01","Grainger")</f>
+        <v>Grainger</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="22">
+        <v>1.23</v>
+      </c>
+      <c r="I4" s="20">
+        <f>H4*C4</f>
+        <v>2.46</v>
+      </c>
+      <c r="J4" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="K4" s="23">
+        <f>C4*J4</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="19">
+        <v>2</v>
+      </c>
+      <c r="D5" s="19">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="20" t="str">
+        <f>HYPERLINK("https://www.grainger.com/product/LASCO-PVC-Male-Adapter-22FJ19","Grainger")</f>
+        <v>Grainger</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="22">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I5" s="20">
+        <v>11.36</v>
+      </c>
+      <c r="J5" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="K5" s="23">
+        <f>C5*J5</f>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="19">
+        <v>2</v>
+      </c>
+      <c r="D6" s="19">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="20" t="str">
+        <f>HYPERLINK("https://www.grainger.com/product/LASCO-PVC-Elbow-22FJ74?cm_sp=Home-_-MyPurchasedProducts-_-22FJ74&amp;cm_vc=HPMPPZ","Grainger")</f>
+        <v>Grainger</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="22">
+        <v>0.66</v>
+      </c>
+      <c r="I6" s="20">
+        <f>H6*C6</f>
+        <v>1.32</v>
+      </c>
+      <c r="J6" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="K6" s="23">
+        <f>C6*J6</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="26">
+        <v>1</v>
+      </c>
+      <c r="D7" s="26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="27" t="str">
+        <f>HYPERLINK("https://www.grainger.com/product/LASCO-PVC-Union-22FM79","Grainger")</f>
+        <v>Grainger</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="29">
+        <v>2.78</v>
+      </c>
+      <c r="I7" s="27">
+        <v>11.36</v>
+      </c>
+      <c r="J7" s="30">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K7" s="30">
+        <f>C7*J7</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="19">
+        <v>2</v>
+      </c>
+      <c r="D8" s="19">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="20" t="str">
+        <f>HYPERLINK("https://www.grainger.com/product/LASCO-PVC-Street-Elbow-22FJ98","Grainger")</f>
+        <v>Grainger</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="22">
+        <v>0.97</v>
+      </c>
+      <c r="I8" s="20">
+        <f>H8*C8</f>
+        <v>1.94</v>
+      </c>
+      <c r="J8" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="K8" s="23">
+        <f>C8*J8</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="26">
+        <v>2</v>
+      </c>
+      <c r="D9" s="26">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="27" t="str">
+        <f>HYPERLINK("https://www.grainger.com/product/GF-PIPING-SYSTEMS-PVC-Union-11W267","Grainger")</f>
+        <v>Grainger</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="29">
+        <v>5.97</v>
+      </c>
+      <c r="I9" s="27">
+        <f>C9*H9</f>
+        <v>11.94</v>
+      </c>
+      <c r="J9" s="30">
+        <v>0.11</v>
+      </c>
+      <c r="K9" s="30">
+        <f>C9*J9</f>
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="26">
+        <v>1</v>
+      </c>
+      <c r="D10" s="26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="27" t="str">
+        <f>HYPERLINK("https://www.homedepot.com/p/1-2-in-Compression-x-1-2-in-FIP-x-12-in-Braided-Polymer-Faucet-Connector-B3-12A-F/100143862","Home Depot")</f>
+        <v>Home Depot</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="29">
+        <v>5.98</v>
+      </c>
+      <c r="I10" s="27">
+        <f>H10*C10</f>
+        <v>5.98</v>
+      </c>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+    </row>
+    <row r="11" spans="1:11" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="26">
+        <v>1</v>
+      </c>
+      <c r="D11" s="26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="27" t="str">
+        <f>HYPERLINK("https://www.homedepot.com/p/BrassCraft-1-2-in-Compression-x-1-2-in-FIP-x-16-in-Braided-Polymer-Faucet-Connector-B3-16A-F/100148838","Home Depot")</f>
+        <v>Home Depot</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="29">
+        <v>6.47</v>
+      </c>
+      <c r="I11" s="27">
+        <f>H11*C11</f>
+        <v>6.47</v>
+      </c>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+    </row>
+    <row r="12" spans="1:11" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="19">
+        <v>1</v>
+      </c>
+      <c r="D12" s="19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="20" t="str">
+        <f>HYPERLINK("https://www.homedepot.com/p/Everbilt-1-2-in-x-1-4-in-Brass-MPT-x-MHT-Boiler-Drain-VBDQTRC3EB/205811822","Home Depot")</f>
+        <v>Home Depot</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="22">
+        <v>8.9</v>
+      </c>
+      <c r="I12" s="20">
+        <f>H12*C12</f>
+        <v>8.9</v>
+      </c>
+      <c r="J12" s="23">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K12" s="23">
+        <f>C12*J12</f>
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="26">
+        <v>1</v>
+      </c>
+      <c r="D13" s="26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="27" t="str">
+        <f>HYPERLINK("https://www.homedepot.com/p/Simpson-Strong-Tie-ZMAX-18-Gauge-Galvanized-Steel-Angle-A21Z/100375047","Home Depot")</f>
+        <v>Home Depot</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="29">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I13" s="27">
+        <f>C13*H13</f>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="J13" s="30">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="K13" s="30">
+        <f>C13*J13</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="19">
+        <v>1</v>
+      </c>
+      <c r="D14" s="19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="20" t="str">
+        <f>HYPERLINK("https://www.matcodist.com/plant-distribution-cartindustrial-rolling-rack-horticulture-cart-nursery-cartplant-cart-flower-cart-greenhouse-transportation-cart","Matco")</f>
+        <v>Matco</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="22">
+        <v>237</v>
+      </c>
+      <c r="I14" s="20">
+        <f>H14*C14</f>
+        <v>237</v>
+      </c>
+      <c r="J14" s="23">
+        <v>60</v>
+      </c>
+      <c r="K14" s="23">
+        <f>C14*J14</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="19">
+        <v>2</v>
+      </c>
+      <c r="D15" s="19">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="20" t="str">
+        <f>HYPERLINK("https://www.mcmaster.com/#4061t163/=1afszoi","McMaster Carr")</f>
+        <v>McMaster Carr</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="22">
+        <v>11.36</v>
+      </c>
+      <c r="I15" s="20">
+        <v>11.36</v>
+      </c>
+      <c r="J15" s="23">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="K15" s="23">
+        <f>C15*J15</f>
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="19">
+        <v>2</v>
+      </c>
+      <c r="D16" s="19">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="20" t="str">
+        <f>HYPERLINK("https://www.mcmaster.com/#3185k112/=1aft071","McMaster Carr")</f>
+        <v>McMaster Carr</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="22">
+        <v>0.44</v>
+      </c>
+      <c r="I16" s="20">
+        <f>H16*C16</f>
+        <v>0.88</v>
+      </c>
+      <c r="J16" s="23">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K16" s="23">
+        <f>C16*J16</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="19">
+        <v>1</v>
+      </c>
+      <c r="D17" s="19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="20" t="str">
+        <f>HYPERLINK("https://www.mcmaster.com/#9930k63/=1aft65a","McMaster Carr")</f>
+        <v>McMaster Carr</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="22">
+        <v>214.79</v>
+      </c>
+      <c r="I17" s="20">
+        <f>C17*H17</f>
+        <v>214.79</v>
+      </c>
+      <c r="J17" s="23">
+        <v>8.4</v>
+      </c>
+      <c r="K17" s="23">
+        <f>C17*J17</f>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="26">
+        <v>3</v>
+      </c>
+      <c r="D18" s="26">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="27" t="str">
+        <f>HYPERLINK("https://www.mscdirect.com/product/details/08802845","MSCDirect")</f>
+        <v>MSCDirect</v>
+      </c>
+      <c r="G18" s="28">
+        <v>8802845</v>
+      </c>
+      <c r="H18" s="29">
+        <v>0.79</v>
+      </c>
+      <c r="I18" s="27">
+        <f>H18*C18</f>
+        <v>2.37</v>
+      </c>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+    </row>
+    <row r="19" spans="1:11" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="26">
+        <v>1</v>
+      </c>
+      <c r="D19" s="26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="27" t="str">
+        <f>HYPERLINK("https://www.mscdirect.com/product/details/05726468","MSCDirect")</f>
+        <v>MSCDirect</v>
+      </c>
+      <c r="G19" s="28">
+        <v>5726468</v>
+      </c>
+      <c r="H19" s="29">
+        <v>0.85</v>
+      </c>
+      <c r="I19" s="27">
+        <f>H19*C19</f>
+        <v>0.85</v>
+      </c>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+    </row>
+    <row r="20" spans="1:11" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="26">
+        <v>1</v>
+      </c>
+      <c r="D20" s="26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="27" t="str">
+        <f>HYPERLINK("https://www.mscdirect.com/product/details/08803066","MSCDirect")</f>
+        <v>MSCDirect</v>
+      </c>
+      <c r="G20" s="28">
+        <v>8803066</v>
+      </c>
+      <c r="H20" s="29">
+        <v>0.8</v>
+      </c>
+      <c r="I20" s="27">
+        <v>11.36</v>
+      </c>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+    </row>
+    <row r="21" spans="1:11" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="26">
+        <v>1</v>
+      </c>
+      <c r="D21" s="26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="27" t="str">
+        <f>HYPERLINK("https://www.mscdirect.com/product/details/50580885","MSCDirect")</f>
+        <v>MSCDirect</v>
+      </c>
+      <c r="G21" s="28">
+        <v>50580885</v>
+      </c>
+      <c r="H21" s="29">
+        <v>0.99</v>
+      </c>
+      <c r="I21" s="27">
+        <f>H21*C21</f>
+        <v>0.99</v>
+      </c>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+    </row>
+    <row r="22" spans="1:11" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="26">
+        <v>3</v>
+      </c>
+      <c r="D22" s="26">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="27" t="str">
+        <f>HYPERLINK("https://www.mscdirect.com/product/details/08802852","MSCDirect")</f>
+        <v>MSCDirect</v>
+      </c>
+      <c r="G22" s="28">
+        <v>8802852</v>
+      </c>
+      <c r="H22" s="29">
+        <v>0.85</v>
+      </c>
+      <c r="I22" s="27">
+        <f>C22*H22</f>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30">
+        <f>C22*J22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="26">
+        <v>1</v>
+      </c>
+      <c r="D23" s="26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="27" t="str">
+        <f>HYPERLINK("https://www.mscdirect.com/product/details/05726484","MSCDirect")</f>
+        <v>MSCDirect</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" s="29">
+        <v>1.05</v>
+      </c>
+      <c r="I23" s="27">
+        <f>C23*H23</f>
+        <v>1.05</v>
+      </c>
+      <c r="J23" s="30">
+        <v>0.18</v>
+      </c>
+      <c r="K23" s="30">
+        <f>C23*J23</f>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19">
+        <v>1</v>
+      </c>
+      <c r="D24" s="19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" s="22">
+        <v>73.87</v>
+      </c>
+      <c r="I24" s="20">
+        <f>C24*H24</f>
+        <v>73.87</v>
+      </c>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+    </row>
+    <row r="25" spans="1:11" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="str">
+        <f>HYPERLINK("https://www.mscdirect.com/product/details/67725085","#6 standoffs")</f>
+        <v>#6 standoffs</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+    </row>
+    <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+    </row>
+    <row r="27" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" display="https://www.amazon.com/dp/B00CJIBMIK/ref=asc_df_B00CJIBMIK5482529/?tag=hyprod-20&amp;creative=394997&amp;creativeASIN=B00CJIBMIK&amp;linkCode=df0&amp;hvadid=167148561991&amp;hvpos=1o1&amp;hvnetw=g&amp;hvrand=6662302602102131996&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9001933&amp;hvtargid=pla-307268360582" xr:uid="{308D2051-71C9-9545-A9CE-9F75703CFDC2}"/>
+  </hyperlinks>
+  <printOptions horizontalCentered="1" headings="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE201083-41FC-AF4D-ABB7-9369055BFD43}">
   <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="13" zeroHeight="1" x14ac:dyDescent="0.15"/>
@@ -1578,40 +2709,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15"/>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15"/>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A7" s="15">
+      <c r="A7" s="14">
         <v>43188</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="169" x14ac:dyDescent="0.15">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15"/>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A10" s="14">
+        <v>43283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A11" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15"/>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15"/>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
hid archived column in fs-rack bom
</commit_message>
<xml_diff>
--- a/prj/fs-rack/v2.0/fs_rack_bom_2.0.xlsx
+++ b/prj/fs-rack/v2.0/fs_rack_bom_2.0.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsavas/Documents/git/openag-mechanical/prj/fs-rack/v2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{182C0AED-D212-C640-8E25-1B23AB07D4AA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1D17EDB1-7B2F-0A49-87AD-4386FC8FEF69}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_fs_rack_bom" sheetId="2" r:id="rId1"/>
-    <sheet name="container03" sheetId="5" r:id="rId2"/>
+    <sheet name="container03" sheetId="5" state="hidden" r:id="rId2"/>
     <sheet name="_meta" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -743,9 +743,9 @@
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1:J1048576"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.15"/>
@@ -830,7 +830,7 @@
         <v>0.41</v>
       </c>
       <c r="K2" s="11">
-        <f>C2*J2</f>
+        <f t="shared" ref="K2:K10" si="0">C2*J2</f>
         <v>0.41</v>
       </c>
     </row>
@@ -843,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="7">
-        <f t="shared" ref="D3:D25" si="0">C3*6</f>
+        <f t="shared" ref="D3:D25" si="1">C3*6</f>
         <v>6</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -866,7 +866,7 @@
         <v>10.8</v>
       </c>
       <c r="K3" s="11">
-        <f>C3*J3</f>
+        <f t="shared" si="0"/>
         <v>10.8</v>
       </c>
     </row>
@@ -881,7 +881,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -905,7 +905,7 @@
         <v>0.1</v>
       </c>
       <c r="K4" s="11">
-        <f>C4*J4</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -920,7 +920,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -943,7 +943,7 @@
         <v>0.03</v>
       </c>
       <c r="K5" s="11">
-        <f>C5*J5</f>
+        <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
     </row>
@@ -958,7 +958,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -982,7 +982,7 @@
         <v>0.05</v>
       </c>
       <c r="K6" s="11">
-        <f>C6*J6</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
@@ -997,7 +997,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -1020,7 +1020,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K7" s="11">
-        <f>C7*J7</f>
+        <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -1059,7 +1059,7 @@
         <v>0.05</v>
       </c>
       <c r="K8" s="11">
-        <f>C8*J8</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
@@ -1074,7 +1074,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -1098,7 +1098,7 @@
         <v>0.2</v>
       </c>
       <c r="K9" s="11">
-        <f>C9*J9</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -1135,7 +1135,7 @@
         <v>0.11</v>
       </c>
       <c r="K10" s="11">
-        <f>C10*J10</f>
+        <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
     </row>
@@ -1150,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -1184,7 +1184,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -1218,7 +1218,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -1242,7 +1242,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="K13" s="11">
-        <f>C13*J13</f>
+        <f t="shared" ref="K13:K18" si="2">C13*J13</f>
         <v>0.28999999999999998</v>
       </c>
     </row>
@@ -1255,7 +1255,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -1279,7 +1279,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="K14" s="11">
-        <f>C14*J14</f>
+        <f t="shared" si="2"/>
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
@@ -1294,7 +1294,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1318,7 +1318,7 @@
         <v>60</v>
       </c>
       <c r="K15" s="11">
-        <f>C15*J15</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
     </row>
@@ -1333,7 +1333,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -1356,7 +1356,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="K16" s="11">
-        <f>C16*J16</f>
+        <f t="shared" si="2"/>
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
@@ -1371,7 +1371,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -1395,7 +1395,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="K17" s="11">
-        <f>C17*J17</f>
+        <f t="shared" si="2"/>
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -1410,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -1434,7 +1434,7 @@
         <v>8.4</v>
       </c>
       <c r="K18" s="11">
-        <f>C18*J18</f>
+        <f t="shared" si="2"/>
         <v>8.4</v>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
         <v>3</v>
       </c>
       <c r="D19" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -1483,7 +1483,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -1517,7 +1517,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -1550,7 +1550,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -1584,7 +1584,7 @@
         <v>3</v>
       </c>
       <c r="D23" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="E23" s="5" t="s">
@@ -1621,7 +1621,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -1658,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E25" s="5" t="s">
@@ -1744,7 +1744,7 @@
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
@@ -1831,7 +1831,7 @@
         <v>0.41</v>
       </c>
       <c r="K2" s="30">
-        <f>C2*J2</f>
+        <f t="shared" ref="K2:K9" si="0">C2*J2</f>
         <v>0.41</v>
       </c>
     </row>
@@ -1844,7 +1844,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="19">
-        <f t="shared" ref="D3:D24" si="0">C3*6</f>
+        <f t="shared" ref="D3:D24" si="1">C3*6</f>
         <v>6</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -1867,7 +1867,7 @@
         <v>10.8</v>
       </c>
       <c r="K3" s="23">
-        <f>C3*J3</f>
+        <f t="shared" si="0"/>
         <v>10.8</v>
       </c>
     </row>
@@ -1882,7 +1882,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -1906,7 +1906,7 @@
         <v>0.1</v>
       </c>
       <c r="K4" s="23">
-        <f>C4*J4</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -1921,7 +1921,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E5" s="17" t="s">
@@ -1944,7 +1944,7 @@
         <v>0.03</v>
       </c>
       <c r="K5" s="23">
-        <f>C5*J5</f>
+        <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
     </row>
@@ -1959,7 +1959,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E6" s="17" t="s">
@@ -1983,7 +1983,7 @@
         <v>0.05</v>
       </c>
       <c r="K6" s="23">
-        <f>C6*J6</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
@@ -1998,7 +1998,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E7" s="24" t="s">
@@ -2021,7 +2021,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K7" s="30">
-        <f>C7*J7</f>
+        <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -2036,7 +2036,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E8" s="17" t="s">
@@ -2060,7 +2060,7 @@
         <v>0.05</v>
       </c>
       <c r="K8" s="23">
-        <f>C8*J8</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
@@ -2073,7 +2073,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E9" s="24" t="s">
@@ -2097,7 +2097,7 @@
         <v>0.11</v>
       </c>
       <c r="K9" s="30">
-        <f>C9*J9</f>
+        <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
     </row>
@@ -2112,7 +2112,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E10" s="24" t="s">
@@ -2146,7 +2146,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E11" s="24" t="s">
@@ -2180,7 +2180,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E12" s="17" t="s">
@@ -2204,7 +2204,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="K12" s="23">
-        <f>C12*J12</f>
+        <f t="shared" ref="K12:K17" si="2">C12*J12</f>
         <v>0.28999999999999998</v>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E13" s="24" t="s">
@@ -2241,7 +2241,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="K13" s="30">
-        <f>C13*J13</f>
+        <f t="shared" si="2"/>
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
@@ -2256,7 +2256,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E14" s="17" t="s">
@@ -2280,7 +2280,7 @@
         <v>60</v>
       </c>
       <c r="K14" s="23">
-        <f>C14*J14</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
     </row>
@@ -2295,7 +2295,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E15" s="17" t="s">
@@ -2318,7 +2318,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="K15" s="23">
-        <f>C15*J15</f>
+        <f t="shared" si="2"/>
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
@@ -2333,7 +2333,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E16" s="17" t="s">
@@ -2357,7 +2357,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="K16" s="23">
-        <f>C16*J16</f>
+        <f t="shared" si="2"/>
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -2372,7 +2372,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E17" s="17" t="s">
@@ -2396,7 +2396,7 @@
         <v>8.4</v>
       </c>
       <c r="K17" s="23">
-        <f>C17*J17</f>
+        <f t="shared" si="2"/>
         <v>8.4</v>
       </c>
     </row>
@@ -2411,7 +2411,7 @@
         <v>3</v>
       </c>
       <c r="D18" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="E18" s="24" t="s">
@@ -2445,7 +2445,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E19" s="24" t="s">
@@ -2479,7 +2479,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E20" s="24" t="s">
@@ -2512,7 +2512,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E21" s="24" t="s">
@@ -2546,7 +2546,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="E22" s="24" t="s">
@@ -2583,7 +2583,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E23" s="24" t="s">
@@ -2620,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E24" s="17" t="s">

</xml_diff>